<commit_message>
Added functionality to save beverage details
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,44 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>53fad91e-c4c8-42f5-a81f-f809f838c37f</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dayly</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Juices</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Coca-Cola</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>16:45:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
I added a cancel button function
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,44 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>34671e4c-d68e-41ff-8a7f-f3ec875dfbe1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>s3Ida</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7UP</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>17:06:19</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented delete functionality for the Delete button, allowing users to remove selected beverage.
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -466,29 +466,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>53fad91e-c4c8-42f5-a81f-f809f838c37f</t>
+          <t>34671e4c-d68e-41ff-8a7f-f3ec875dfbe1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dayly</t>
+          <t>s3Ida</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Juices</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Coca-Cola</t>
+          <t>7UP</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -497,19 +497,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>16:45:10</t>
+          <t>17:06:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>34671e4c-d68e-41ff-8a7f-f3ec875dfbe1</t>
+          <t>32b13210-7cf0-4040-8158-3648e246efed</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>s3Ida</t>
+          <t>,s,xkks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -523,19 +523,19 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-09-13</t>
+          <t>2024-09-14</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>17:06:19</t>
+          <t>12:32:28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored delete_product and delete_beverage into a single function, delete_item, to streamline code and reduce duplication.
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,44 +501,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>32b13210-7cf0-4040-8158-3648e246efed</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>,s,xkks</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7UP</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2024-09-14</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>12:32:28</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented delete functionality for the update button, allowing users to update selcted item
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,19 +485,57 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2" t="n">
         <v>50</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-09-13</t>
+          <t>2024-09-14</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>17:06:19</t>
+          <t>13:05:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>86100910-a497-4f46-a192-4b0daf98da07</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>xksksjd</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Soft Drinks</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7UP</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2024-09-14</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>13:08:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored update_product and update_beverage into a single function, update_itm, to streamline code and reduce deplication.
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>50</v>
@@ -497,7 +497,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>13:05:32</t>
+          <t>13:40:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
i add to the beverage sales section return functionality
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
         <v>50</v>
@@ -523,19 +523,19 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>100</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-09-14</t>
+          <t>2024-09-15</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14:24:23</t>
+          <t>01:01:32</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
i add save functionality in the printer part
</commit_message>
<xml_diff>
--- a/beverage.xlsx
+++ b/beverage.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,44 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2ac21e18-91a2-45af-b5b2-dadf7b7d688c</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dayli</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Juices</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Coca-Cola</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>95</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>18:22:11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>